<commit_message>
Update Team OD- Data for OD v Time.xlsx
Minor edits to OD v time excel
</commit_message>
<xml_diff>
--- a/Week 1/Team OD- Data for OD v Time.xlsx
+++ b/Week 1/Team OD- Data for OD v Time.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f5ea6b64b302b667/Documents/Med/Team-OD_Fermentation-Pract_Data_UoB/Week 1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f5ea6b64b302b667/Documents/Med/Team-OD_Fermentation-Pract_Data_UoB/New folder/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{07FF89B3-496F-4235-A29D-E03C3CDC546C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{07FF89B3-496F-4235-A29D-E03C3CDC546C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B75A2E7B-8D0B-482F-836E-FF98125C3F58}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{681A5516-1CEC-4A1E-A072-B1CCDEA33CD4}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="7">
   <si>
     <t>Real Time</t>
   </si>
@@ -56,12 +56,6 @@
   </si>
   <si>
     <t>Optical Density Graph</t>
-  </si>
-  <si>
-    <t>OD</t>
-  </si>
-  <si>
-    <t>Estimated Protein Production</t>
   </si>
   <si>
     <t>After inducing IPTG</t>
@@ -181,6 +175,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="20" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -196,7 +191,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5895,6 +5889,10 @@
           </cell>
         </row>
         <row r="13">
+          <cell r="B13"/>
+          <cell r="C13"/>
+          <cell r="E13"/>
+          <cell r="F13"/>
           <cell r="H13">
             <v>1445</v>
           </cell>
@@ -5909,6 +5907,12 @@
           </cell>
         </row>
         <row r="14">
+          <cell r="B14"/>
+          <cell r="C14"/>
+          <cell r="E14"/>
+          <cell r="F14"/>
+          <cell r="H14"/>
+          <cell r="I14"/>
           <cell r="K14">
             <v>372</v>
           </cell>
@@ -5917,6 +5921,12 @@
           </cell>
         </row>
         <row r="15">
+          <cell r="B15"/>
+          <cell r="C15"/>
+          <cell r="E15"/>
+          <cell r="F15"/>
+          <cell r="H15"/>
+          <cell r="I15"/>
           <cell r="K15">
             <v>432</v>
           </cell>
@@ -5925,6 +5935,12 @@
           </cell>
         </row>
         <row r="16">
+          <cell r="B16"/>
+          <cell r="C16"/>
+          <cell r="E16"/>
+          <cell r="F16"/>
+          <cell r="H16"/>
+          <cell r="I16"/>
           <cell r="K16">
             <v>1471</v>
           </cell>
@@ -5932,11 +5948,171 @@
             <v>3.27</v>
           </cell>
         </row>
+        <row r="17">
+          <cell r="B17"/>
+          <cell r="C17"/>
+          <cell r="E17"/>
+          <cell r="F17"/>
+          <cell r="H17"/>
+          <cell r="I17"/>
+          <cell r="K17"/>
+          <cell r="L17"/>
+        </row>
+        <row r="18">
+          <cell r="B18"/>
+          <cell r="C18"/>
+          <cell r="E18"/>
+          <cell r="F18"/>
+          <cell r="H18"/>
+          <cell r="I18"/>
+          <cell r="K18"/>
+          <cell r="L18"/>
+        </row>
+        <row r="19">
+          <cell r="B19"/>
+          <cell r="C19"/>
+          <cell r="E19"/>
+          <cell r="F19"/>
+          <cell r="H19"/>
+          <cell r="I19"/>
+          <cell r="K19"/>
+          <cell r="L19"/>
+        </row>
+        <row r="20">
+          <cell r="B20"/>
+          <cell r="C20"/>
+          <cell r="E20"/>
+          <cell r="F20"/>
+          <cell r="H20"/>
+          <cell r="I20"/>
+          <cell r="K20"/>
+          <cell r="L20"/>
+        </row>
+        <row r="21">
+          <cell r="B21"/>
+          <cell r="C21"/>
+          <cell r="E21"/>
+          <cell r="F21"/>
+          <cell r="H21"/>
+          <cell r="I21"/>
+          <cell r="K21"/>
+          <cell r="L21"/>
+        </row>
+        <row r="22">
+          <cell r="B22"/>
+          <cell r="C22"/>
+          <cell r="E22"/>
+          <cell r="F22"/>
+          <cell r="H22"/>
+          <cell r="I22"/>
+          <cell r="K22"/>
+          <cell r="L22"/>
+        </row>
+        <row r="23">
+          <cell r="B23"/>
+          <cell r="C23"/>
+          <cell r="E23"/>
+          <cell r="F23"/>
+          <cell r="H23"/>
+          <cell r="I23"/>
+          <cell r="K23"/>
+          <cell r="L23"/>
+        </row>
+        <row r="24">
+          <cell r="B24"/>
+          <cell r="C24"/>
+          <cell r="E24"/>
+          <cell r="F24"/>
+          <cell r="H24"/>
+          <cell r="I24"/>
+          <cell r="K24"/>
+          <cell r="L24"/>
+        </row>
+        <row r="25">
+          <cell r="B25"/>
+          <cell r="C25"/>
+          <cell r="E25"/>
+          <cell r="F25"/>
+          <cell r="H25"/>
+          <cell r="I25"/>
+          <cell r="K25"/>
+          <cell r="L25"/>
+        </row>
+        <row r="26">
+          <cell r="B26"/>
+          <cell r="C26"/>
+          <cell r="E26"/>
+          <cell r="F26"/>
+          <cell r="H26"/>
+          <cell r="I26"/>
+          <cell r="K26"/>
+          <cell r="L26"/>
+        </row>
+        <row r="27">
+          <cell r="B27"/>
+          <cell r="C27"/>
+          <cell r="E27"/>
+          <cell r="F27"/>
+          <cell r="H27"/>
+          <cell r="I27"/>
+          <cell r="K27"/>
+          <cell r="L27"/>
+        </row>
+        <row r="28">
+          <cell r="B28"/>
+          <cell r="C28"/>
+          <cell r="E28"/>
+          <cell r="F28"/>
+          <cell r="H28"/>
+          <cell r="I28"/>
+          <cell r="K28"/>
+          <cell r="L28"/>
+        </row>
+        <row r="29">
+          <cell r="B29"/>
+          <cell r="C29"/>
+          <cell r="E29"/>
+          <cell r="F29"/>
+          <cell r="H29"/>
+          <cell r="I29"/>
+          <cell r="K29"/>
+          <cell r="L29"/>
+        </row>
+        <row r="30">
+          <cell r="B30"/>
+          <cell r="C30"/>
+          <cell r="E30"/>
+          <cell r="F30"/>
+          <cell r="H30"/>
+          <cell r="I30"/>
+          <cell r="K30"/>
+          <cell r="L30"/>
+        </row>
+        <row r="31">
+          <cell r="B31"/>
+          <cell r="C31"/>
+          <cell r="E31"/>
+          <cell r="F31"/>
+          <cell r="H31"/>
+          <cell r="I31"/>
+          <cell r="K31"/>
+          <cell r="L31"/>
+        </row>
+        <row r="32">
+          <cell r="B32"/>
+          <cell r="C32"/>
+          <cell r="E32"/>
+          <cell r="F32"/>
+          <cell r="H32"/>
+          <cell r="I32"/>
+          <cell r="K32"/>
+          <cell r="L32"/>
+        </row>
       </sheetData>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -6239,10 +6415,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{679BF6B7-5D78-49EA-AB75-840F077FDEF6}">
-  <dimension ref="A1:AE32"/>
+  <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="V44" sqref="V44"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="AD3" sqref="AD3:AE7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6265,23 +6441,23 @@
     <col min="31" max="31" width="28.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" ht="21" x14ac:dyDescent="0.4">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.4">
+      <c r="A1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
     </row>
-    <row r="3" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -6318,14 +6494,8 @@
       <c r="L3" s="1">
         <v>1</v>
       </c>
-      <c r="AD3" t="s">
-        <v>6</v>
-      </c>
-      <c r="AE3" t="s">
-        <v>7</v>
-      </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>0.4381944444444445</v>
       </c>
@@ -6362,14 +6532,8 @@
       <c r="L4" s="3">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="AD4">
-        <v>4</v>
-      </c>
-      <c r="AE4">
-        <v>0.4</v>
-      </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>0.48055555555555557</v>
       </c>
@@ -6406,14 +6570,8 @@
       <c r="L5" s="3">
         <v>5.8999999999999997E-2</v>
       </c>
-      <c r="AD5">
-        <v>2.5</v>
-      </c>
-      <c r="AE5">
-        <v>0.6</v>
-      </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>0.5</v>
       </c>
@@ -6450,14 +6608,8 @@
       <c r="L6" s="3">
         <v>0.29199999999999998</v>
       </c>
-      <c r="AD6">
-        <v>2</v>
-      </c>
-      <c r="AE6">
-        <v>0.8</v>
-      </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>0.52083333333333337</v>
       </c>
@@ -6494,14 +6646,8 @@
       <c r="L7" s="3">
         <v>0.48899999999999999</v>
       </c>
-      <c r="AD7">
-        <v>3.3</v>
-      </c>
-      <c r="AE7">
-        <v>1</v>
-      </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>0.52847222222222223</v>
       </c>
@@ -6539,7 +6685,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="G9" s="2">
         <v>0.53819444444444442</v>
       </c>
@@ -6559,7 +6705,7 @@
         <v>0.83299999999999996</v>
       </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="J10" s="2">
         <v>0.54861111111111105</v>
       </c>
@@ -6570,7 +6716,7 @@
         <v>0.88600000000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="J11" s="2">
         <v>0.55902777777777779</v>
       </c>
@@ -6581,7 +6727,7 @@
         <v>0.93600000000000005</v>
       </c>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="J12" s="2">
         <v>0.56597222222222221</v>
       </c>
@@ -6592,37 +6738,37 @@
         <v>1.0029999999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A13" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="8"/>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A14" s="9"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="10"/>
-      <c r="L14" s="10"/>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14" s="10"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="11"/>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>0.58958333333333335</v>
       </c>
@@ -6660,7 +6806,7 @@
         <v>1.97</v>
       </c>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>0.63124999999999998</v>
       </c>
@@ -6775,200 +6921,200 @@
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A19" s="11"/>
-      <c r="B19" s="11"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="11"/>
-      <c r="J19" s="11"/>
-      <c r="K19" s="11"/>
-      <c r="L19" s="11"/>
+      <c r="A19" s="6"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="6"/>
+      <c r="L19" s="6"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A20" s="11"/>
-      <c r="B20" s="11"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="11"/>
-      <c r="J20" s="11"/>
-      <c r="K20" s="11"/>
-      <c r="L20" s="11"/>
+      <c r="A20" s="6"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="6"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A21" s="11"/>
-      <c r="B21" s="11"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="11"/>
-      <c r="J21" s="11"/>
-      <c r="K21" s="11"/>
-      <c r="L21" s="11"/>
+      <c r="A21" s="6"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="6"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A22" s="11"/>
-      <c r="B22" s="11"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="11"/>
-      <c r="I22" s="11"/>
-      <c r="J22" s="11"/>
-      <c r="K22" s="11"/>
-      <c r="L22" s="11"/>
+      <c r="A22" s="6"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="6"/>
+      <c r="L22" s="6"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A23" s="11"/>
-      <c r="B23" s="11"/>
-      <c r="C23" s="11"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="11"/>
-      <c r="H23" s="11"/>
-      <c r="I23" s="11"/>
-      <c r="J23" s="11"/>
-      <c r="K23" s="11"/>
-      <c r="L23" s="11"/>
+      <c r="A23" s="6"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="6"/>
+      <c r="L23" s="6"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A24" s="11"/>
-      <c r="B24" s="11"/>
-      <c r="C24" s="11"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="11"/>
-      <c r="H24" s="11"/>
-      <c r="I24" s="11"/>
-      <c r="J24" s="11"/>
-      <c r="K24" s="11"/>
-      <c r="L24" s="11"/>
+      <c r="A24" s="6"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="6"/>
+      <c r="L24" s="6"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A25" s="11"/>
-      <c r="B25" s="11"/>
-      <c r="C25" s="11"/>
-      <c r="D25" s="11"/>
-      <c r="E25" s="11"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="11"/>
-      <c r="H25" s="11"/>
-      <c r="I25" s="11"/>
-      <c r="J25" s="11"/>
-      <c r="K25" s="11"/>
-      <c r="L25" s="11"/>
+      <c r="A25" s="6"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="6"/>
+      <c r="K25" s="6"/>
+      <c r="L25" s="6"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A26" s="11"/>
-      <c r="B26" s="11"/>
-      <c r="C26" s="11"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="11"/>
-      <c r="F26" s="11"/>
-      <c r="G26" s="11"/>
-      <c r="H26" s="11"/>
-      <c r="I26" s="11"/>
-      <c r="J26" s="11"/>
-      <c r="K26" s="11"/>
-      <c r="L26" s="11"/>
+      <c r="A26" s="6"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="6"/>
+      <c r="K26" s="6"/>
+      <c r="L26" s="6"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A27" s="11"/>
-      <c r="B27" s="11"/>
-      <c r="C27" s="11"/>
-      <c r="D27" s="11"/>
-      <c r="E27" s="11"/>
-      <c r="F27" s="11"/>
-      <c r="G27" s="11"/>
-      <c r="H27" s="11"/>
-      <c r="I27" s="11"/>
-      <c r="J27" s="11"/>
-      <c r="K27" s="11"/>
-      <c r="L27" s="11"/>
+      <c r="A27" s="6"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
+      <c r="I27" s="6"/>
+      <c r="J27" s="6"/>
+      <c r="K27" s="6"/>
+      <c r="L27" s="6"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A28" s="11"/>
-      <c r="B28" s="11"/>
-      <c r="C28" s="11"/>
-      <c r="D28" s="11"/>
-      <c r="E28" s="11"/>
-      <c r="F28" s="11"/>
-      <c r="G28" s="11"/>
-      <c r="H28" s="11"/>
-      <c r="I28" s="11"/>
-      <c r="J28" s="11"/>
-      <c r="K28" s="11"/>
-      <c r="L28" s="11"/>
+      <c r="A28" s="6"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="6"/>
+      <c r="J28" s="6"/>
+      <c r="K28" s="6"/>
+      <c r="L28" s="6"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A29" s="11"/>
-      <c r="B29" s="11"/>
-      <c r="C29" s="11"/>
-      <c r="D29" s="11"/>
-      <c r="E29" s="11"/>
-      <c r="F29" s="11"/>
-      <c r="G29" s="11"/>
-      <c r="H29" s="11"/>
-      <c r="I29" s="11"/>
-      <c r="J29" s="11"/>
-      <c r="K29" s="11"/>
-      <c r="L29" s="11"/>
+      <c r="A29" s="6"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
+      <c r="I29" s="6"/>
+      <c r="J29" s="6"/>
+      <c r="K29" s="6"/>
+      <c r="L29" s="6"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A30" s="11"/>
-      <c r="B30" s="11"/>
-      <c r="C30" s="11"/>
-      <c r="D30" s="11"/>
-      <c r="E30" s="11"/>
-      <c r="F30" s="11"/>
-      <c r="G30" s="11"/>
-      <c r="H30" s="11"/>
-      <c r="I30" s="11"/>
-      <c r="J30" s="11"/>
-      <c r="K30" s="11"/>
-      <c r="L30" s="11"/>
+      <c r="A30" s="6"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="6"/>
+      <c r="I30" s="6"/>
+      <c r="J30" s="6"/>
+      <c r="K30" s="6"/>
+      <c r="L30" s="6"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A31" s="11"/>
-      <c r="B31" s="11"/>
-      <c r="C31" s="11"/>
-      <c r="D31" s="11"/>
-      <c r="E31" s="11"/>
-      <c r="F31" s="11"/>
-      <c r="G31" s="11"/>
-      <c r="H31" s="11"/>
-      <c r="I31" s="11"/>
-      <c r="J31" s="11"/>
-      <c r="K31" s="11"/>
-      <c r="L31" s="11"/>
+      <c r="A31" s="6"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
+      <c r="I31" s="6"/>
+      <c r="J31" s="6"/>
+      <c r="K31" s="6"/>
+      <c r="L31" s="6"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A32" s="11"/>
-      <c r="B32" s="11"/>
-      <c r="C32" s="11"/>
-      <c r="D32" s="11"/>
-      <c r="E32" s="11"/>
-      <c r="F32" s="11"/>
-      <c r="G32" s="11"/>
-      <c r="H32" s="11"/>
-      <c r="I32" s="11"/>
-      <c r="J32" s="11"/>
-      <c r="K32" s="11"/>
-      <c r="L32" s="11"/>
+      <c r="A32" s="6"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="6"/>
+      <c r="I32" s="6"/>
+      <c r="J32" s="6"/>
+      <c r="K32" s="6"/>
+      <c r="L32" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -6982,21 +7128,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005724447BD77D1F4AB2324D8F6F5BF2E6" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0e825634e906f572a5eacb9cb3d566c8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="2dd46c47-06b0-4a50-b78f-8abce2fae7a5" xmlns:ns4="46715210-e6c3-4eca-8675-f906fa2a9ce0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b233c504b3d4196d9db9d4d65f966814" ns3:_="" ns4:_="">
     <xsd:import namespace="2dd46c47-06b0-4a50-b78f-8abce2fae7a5"/>
@@ -7219,10 +7350,36 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F31972C3-9453-461B-B022-516B3B8151A0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{88EA95A7-D48C-4798-A6CD-6AE7EB3D6817}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="2dd46c47-06b0-4a50-b78f-8abce2fae7a5"/>
+    <ds:schemaRef ds:uri="46715210-e6c3-4eca-8675-f906fa2a9ce0"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -7245,20 +7402,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{88EA95A7-D48C-4798-A6CD-6AE7EB3D6817}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F31972C3-9453-461B-B022-516B3B8151A0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="2dd46c47-06b0-4a50-b78f-8abce2fae7a5"/>
-    <ds:schemaRef ds:uri="46715210-e6c3-4eca-8675-f906fa2a9ce0"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>